<commit_message>
Add Test Case Table for Black-box Testing
</commit_message>
<xml_diff>
--- a/CP_Config/4_Implementation_&_Testing/Requisites/Testing/BlackBoxTesting/Test Cases Table.xlsx
+++ b/CP_Config/4_Implementation_&_Testing/Requisites/Testing/BlackBoxTesting/Test Cases Table.xlsx
@@ -740,20 +740,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>